<commit_message>
work plan and proposal
</commit_message>
<xml_diff>
--- a/workplan.xlsx
+++ b/workplan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -47,9 +47,6 @@
     <t>December</t>
   </si>
   <si>
-    <t>February</t>
-  </si>
-  <si>
     <t>March</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
   </si>
   <si>
     <t>Scope definition</t>
-  </si>
-  <si>
-    <t>Proposal</t>
   </si>
   <si>
     <t>Capture Requirements</t>
@@ -172,6 +166,15 @@
   </si>
   <si>
     <t>Acceptance and Deployment</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>w3</t>
+  </si>
+  <si>
+    <t>Drafting Proposal and Presentation</t>
   </si>
 </sst>
 </file>
@@ -187,12 +190,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -207,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +233,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,88 +526,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AQ35"/>
+  <dimension ref="A2:AP35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="X1" sqref="X1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="33.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="7" width="5.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="16" width="6.7109375" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" customWidth="1"/>
+    <col min="21" max="21" width="5.28515625" customWidth="1"/>
+    <col min="22" max="22" width="6" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" customWidth="1"/>
+    <col min="24" max="24" width="5.140625" customWidth="1"/>
+    <col min="25" max="25" width="5.7109375" customWidth="1"/>
+    <col min="26" max="26" width="5.140625" customWidth="1"/>
+    <col min="27" max="30" width="5.5703125" customWidth="1"/>
+    <col min="31" max="31" width="5.28515625" customWidth="1"/>
+    <col min="32" max="32" width="5.140625" customWidth="1"/>
+    <col min="33" max="33" width="5.7109375" customWidth="1"/>
+    <col min="34" max="34" width="4.85546875" customWidth="1"/>
+    <col min="35" max="35" width="5" customWidth="1"/>
+    <col min="36" max="36" width="5.28515625" customWidth="1"/>
+    <col min="37" max="37" width="5.42578125" customWidth="1"/>
+    <col min="38" max="38" width="5.85546875" customWidth="1"/>
+    <col min="39" max="39" width="5.140625" customWidth="1"/>
+    <col min="40" max="40" width="4.7109375" customWidth="1"/>
+    <col min="41" max="41" width="5.28515625" customWidth="1"/>
+    <col min="42" max="42" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1" t="s">
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1" t="s">
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1" t="s">
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1" t="s">
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-    </row>
-    <row r="3" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="AN2" s="6"/>
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="6"/>
+    </row>
+    <row r="3" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -593,359 +642,398 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="N3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="R3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="U3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="V3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U3" t="s">
+      <c r="Z3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="V3" t="s">
-        <v>24</v>
-      </c>
-      <c r="W3" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="AA3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AD3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB3" t="s">
+      <c r="AE3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AH3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF3" t="s">
+      <c r="AI3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AL3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AJ3" t="s">
+      <c r="AM3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AP3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>23</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>4.2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>5.0999999999999996</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>5.2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>5.3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>5.4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="P15" s="9"/>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5.6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>6.1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="R18" s="9"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>6.2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="R19" s="10"/>
+      <c r="S19" s="11"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>6.3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="R20" s="12"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>6.4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>6.5</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>6.6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>7.1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>7.2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>7.3</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>8</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>8.1</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>8.1999999999999993</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>8.4</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -953,7 +1041,7 @@
         <v>8.5</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -961,7 +1049,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -969,21 +1057,31 @@
         <v>10</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="AF2:AI2"/>
-    <mergeCell ref="AJ2:AM2"/>
-    <mergeCell ref="AN2:AQ2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:W2"/>
+  <mergeCells count="20">
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="R17:W17"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>